<commit_message>
ajuste en etl.py para poder extraer el codigo de la pregunta y continuar el proceso de ejecucion, se agrega archuivo debug para poder hacer el los ajustes usando jupyter
</commit_message>
<xml_diff>
--- a/catalogos/catalogo_1.xlsx
+++ b/catalogos/catalogo_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berse\Documents\Caramelo escaso\caramelo\misc\catalogos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berse\Documents\Caramelo escaso\caramelo\catalogos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D2ECA0-FF44-414E-A904-2C0B35248FAF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985BCBC2-FBE5-47E1-AB05-F589A5006ECD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{855AF920-00D3-496D-A6BC-53AC25B09997}"/>
+    <workbookView xWindow="0" yWindow="390" windowWidth="20490" windowHeight="10920" xr2:uid="{855AF920-00D3-496D-A6BC-53AC25B09997}"/>
   </bookViews>
   <sheets>
     <sheet name="Catalogo_1" sheetId="1" r:id="rId1"/>
@@ -132,789 +132,9 @@
     <t>Identificador_pregunta</t>
   </si>
   <si>
-    <t>y1</t>
-  </si>
-  <si>
-    <t>y2</t>
-  </si>
-  <si>
-    <t>y3</t>
-  </si>
-  <si>
-    <t>y4</t>
-  </si>
-  <si>
-    <t>y5</t>
-  </si>
-  <si>
-    <t>y6</t>
-  </si>
-  <si>
-    <t>y7</t>
-  </si>
-  <si>
-    <t>y8</t>
-  </si>
-  <si>
-    <t>y9</t>
-  </si>
-  <si>
-    <t>y10</t>
-  </si>
-  <si>
-    <t>y11</t>
-  </si>
-  <si>
-    <t>y12</t>
-  </si>
-  <si>
-    <t>y13</t>
-  </si>
-  <si>
-    <t>y14</t>
-  </si>
-  <si>
-    <t>y15</t>
-  </si>
-  <si>
-    <t>y16</t>
-  </si>
-  <si>
-    <t>y17</t>
-  </si>
-  <si>
-    <t>y18</t>
-  </si>
-  <si>
-    <t>y19</t>
-  </si>
-  <si>
-    <t>y20</t>
-  </si>
-  <si>
-    <t>y21</t>
-  </si>
-  <si>
-    <t>y22</t>
-  </si>
-  <si>
-    <t>y23</t>
-  </si>
-  <si>
-    <t>y24</t>
-  </si>
-  <si>
-    <t>y25</t>
-  </si>
-  <si>
-    <t>y26</t>
-  </si>
-  <si>
-    <t>n27</t>
-  </si>
-  <si>
-    <t>n28</t>
-  </si>
-  <si>
-    <t>n29</t>
-  </si>
-  <si>
-    <t>n30</t>
-  </si>
-  <si>
-    <t>n31</t>
-  </si>
-  <si>
-    <t>n32</t>
-  </si>
-  <si>
-    <t>n33</t>
-  </si>
-  <si>
-    <t>n34</t>
-  </si>
-  <si>
-    <t>n35</t>
-  </si>
-  <si>
-    <t>n36</t>
-  </si>
-  <si>
-    <t>n37</t>
-  </si>
-  <si>
-    <t>n38</t>
-  </si>
-  <si>
-    <t>n39</t>
-  </si>
-  <si>
-    <t>n40</t>
-  </si>
-  <si>
-    <t>n41</t>
-  </si>
-  <si>
-    <t>n42</t>
-  </si>
-  <si>
-    <t>n43</t>
-  </si>
-  <si>
-    <t>n44</t>
-  </si>
-  <si>
-    <t>n45</t>
-  </si>
-  <si>
-    <t>n46</t>
-  </si>
-  <si>
-    <t>n47</t>
-  </si>
-  <si>
-    <t>n48</t>
-  </si>
-  <si>
-    <t>n49</t>
-  </si>
-  <si>
-    <t>n50</t>
-  </si>
-  <si>
-    <t>n51</t>
-  </si>
-  <si>
-    <t>n52</t>
-  </si>
-  <si>
-    <t>n53</t>
-  </si>
-  <si>
-    <t>n54</t>
-  </si>
-  <si>
-    <t>n55</t>
-  </si>
-  <si>
-    <t>n56</t>
-  </si>
-  <si>
-    <t>n57</t>
-  </si>
-  <si>
-    <t>n58</t>
-  </si>
-  <si>
-    <t>n59</t>
-  </si>
-  <si>
-    <t>n60</t>
-  </si>
-  <si>
-    <t>n61</t>
-  </si>
-  <si>
-    <t>n62</t>
-  </si>
-  <si>
-    <t>n63</t>
-  </si>
-  <si>
-    <t>n64</t>
-  </si>
-  <si>
-    <t>n65</t>
-  </si>
-  <si>
-    <t>n66</t>
-  </si>
-  <si>
-    <t>n67</t>
-  </si>
-  <si>
-    <t>n68</t>
-  </si>
-  <si>
-    <t>n69</t>
-  </si>
-  <si>
-    <t>n70</t>
-  </si>
-  <si>
-    <t>n71</t>
-  </si>
-  <si>
-    <t>n72</t>
-  </si>
-  <si>
-    <t>n73</t>
-  </si>
-  <si>
-    <t>n74</t>
-  </si>
-  <si>
-    <t>n75</t>
-  </si>
-  <si>
-    <t>n76</t>
-  </si>
-  <si>
-    <t>n77</t>
-  </si>
-  <si>
-    <t>n78</t>
-  </si>
-  <si>
-    <t>t79</t>
-  </si>
-  <si>
-    <t>t80</t>
-  </si>
-  <si>
-    <t>t81</t>
-  </si>
-  <si>
-    <t>t82</t>
-  </si>
-  <si>
-    <t>t83</t>
-  </si>
-  <si>
-    <t>t84</t>
-  </si>
-  <si>
-    <t>t85</t>
-  </si>
-  <si>
-    <t>t86</t>
-  </si>
-  <si>
-    <t>t87</t>
-  </si>
-  <si>
-    <t>t88</t>
-  </si>
-  <si>
-    <t>t89</t>
-  </si>
-  <si>
-    <t>t90</t>
-  </si>
-  <si>
-    <t>t91</t>
-  </si>
-  <si>
-    <t>t92</t>
-  </si>
-  <si>
-    <t>t93</t>
-  </si>
-  <si>
-    <t>t94</t>
-  </si>
-  <si>
-    <t>t95</t>
-  </si>
-  <si>
-    <t>t96</t>
-  </si>
-  <si>
-    <t>t97</t>
-  </si>
-  <si>
-    <t>t98</t>
-  </si>
-  <si>
-    <t>t99</t>
-  </si>
-  <si>
-    <t>t100</t>
-  </si>
-  <si>
-    <t>t101</t>
-  </si>
-  <si>
-    <t>t102</t>
-  </si>
-  <si>
-    <t>t103</t>
-  </si>
-  <si>
-    <t>t104</t>
-  </si>
-  <si>
-    <t>t105</t>
-  </si>
-  <si>
-    <t>t106</t>
-  </si>
-  <si>
-    <t>t107</t>
-  </si>
-  <si>
-    <t>t108</t>
-  </si>
-  <si>
-    <t>t109</t>
-  </si>
-  <si>
-    <t>t110</t>
-  </si>
-  <si>
-    <t>t111</t>
-  </si>
-  <si>
-    <t>t112</t>
-  </si>
-  <si>
-    <t>t113</t>
-  </si>
-  <si>
-    <t>t114</t>
-  </si>
-  <si>
-    <t>t115</t>
-  </si>
-  <si>
-    <t>t116</t>
-  </si>
-  <si>
-    <t>t117</t>
-  </si>
-  <si>
-    <t>t118</t>
-  </si>
-  <si>
-    <t>t119</t>
-  </si>
-  <si>
-    <t>t120</t>
-  </si>
-  <si>
-    <t>t121</t>
-  </si>
-  <si>
-    <t>t122</t>
-  </si>
-  <si>
-    <t>t123</t>
-  </si>
-  <si>
-    <t>t124</t>
-  </si>
-  <si>
-    <t>t125</t>
-  </si>
-  <si>
-    <t>t126</t>
-  </si>
-  <si>
-    <t>t127</t>
-  </si>
-  <si>
-    <t>t128</t>
-  </si>
-  <si>
-    <t>t129</t>
-  </si>
-  <si>
-    <t>t130</t>
-  </si>
-  <si>
     <t>actuacion</t>
   </si>
   <si>
-    <t>pnt_y1</t>
-  </si>
-  <si>
-    <t>pnt_y2</t>
-  </si>
-  <si>
-    <t>pnt_y3</t>
-  </si>
-  <si>
-    <t>pnt_y4</t>
-  </si>
-  <si>
-    <t>pnt_y5</t>
-  </si>
-  <si>
-    <t>pnt_y6</t>
-  </si>
-  <si>
-    <t>pnt_y7</t>
-  </si>
-  <si>
-    <t>pnt_y8</t>
-  </si>
-  <si>
-    <t>pnt_y9</t>
-  </si>
-  <si>
-    <t>pnt_y10</t>
-  </si>
-  <si>
-    <t>pnt_y11</t>
-  </si>
-  <si>
-    <t>pnt_y12</t>
-  </si>
-  <si>
-    <t>pnt_y13</t>
-  </si>
-  <si>
-    <t>pnt_y14</t>
-  </si>
-  <si>
-    <t>pnt_y15</t>
-  </si>
-  <si>
-    <t>pnt_y16</t>
-  </si>
-  <si>
-    <t>pnt_y17</t>
-  </si>
-  <si>
-    <t>pnt_y18</t>
-  </si>
-  <si>
-    <t>pnt_y19</t>
-  </si>
-  <si>
-    <t>pnt_y20</t>
-  </si>
-  <si>
-    <t>pnt_y21</t>
-  </si>
-  <si>
-    <t>pnt_y22</t>
-  </si>
-  <si>
-    <t>pnt_y23</t>
-  </si>
-  <si>
-    <t>pnt_y24</t>
-  </si>
-  <si>
-    <t>pnt_y25</t>
-  </si>
-  <si>
-    <t>pnt_y26</t>
-  </si>
-  <si>
-    <t>pnt_n27</t>
-  </si>
-  <si>
-    <t>pnt_n28</t>
-  </si>
-  <si>
-    <t>pnt_n29</t>
-  </si>
-  <si>
-    <t>pnt_n30</t>
-  </si>
-  <si>
-    <t>pnt_n31</t>
-  </si>
-  <si>
-    <t>pnt_n32</t>
-  </si>
-  <si>
-    <t>pnt_n33</t>
-  </si>
-  <si>
-    <t>pnt_n34</t>
-  </si>
-  <si>
-    <t>pnt_n35</t>
-  </si>
-  <si>
-    <t>pnt_n36</t>
-  </si>
-  <si>
-    <t>pnt_n37</t>
-  </si>
-  <si>
-    <t>pnt_n38</t>
-  </si>
-  <si>
-    <t>pnt_n39</t>
-  </si>
-  <si>
-    <t>pnt_n40</t>
-  </si>
-  <si>
-    <t>pnt_n41</t>
-  </si>
-  <si>
-    <t>pnt_n42</t>
-  </si>
-  <si>
-    <t>pnt_n43</t>
-  </si>
-  <si>
-    <t>pnt_n44</t>
-  </si>
-  <si>
-    <t>pnt_n45</t>
-  </si>
-  <si>
-    <t>pnt_n46</t>
-  </si>
-  <si>
-    <t>pnt_n47</t>
-  </si>
-  <si>
-    <t>pnt_n48</t>
-  </si>
-  <si>
-    <t>pnt_n49</t>
-  </si>
-  <si>
-    <t>pnt_n50</t>
-  </si>
-  <si>
-    <t>pnt_n51</t>
-  </si>
-  <si>
-    <t>pnt_n52</t>
-  </si>
-  <si>
-    <t>pnt_n53</t>
-  </si>
-  <si>
-    <t>pnt_n54</t>
-  </si>
-  <si>
-    <t>pnt_n55</t>
-  </si>
-  <si>
-    <t>pnt_n56</t>
-  </si>
-  <si>
-    <t>pnt_n57</t>
-  </si>
-  <si>
-    <t>pnt_n58</t>
-  </si>
-  <si>
-    <t>pnt_n59</t>
-  </si>
-  <si>
-    <t>pnt_n60</t>
-  </si>
-  <si>
-    <t>pnt_n61</t>
-  </si>
-  <si>
-    <t>pnt_n62</t>
-  </si>
-  <si>
-    <t>pnt_n63</t>
-  </si>
-  <si>
-    <t>pnt_n64</t>
-  </si>
-  <si>
-    <t>pnt_n65</t>
-  </si>
-  <si>
-    <t>pnt_n66</t>
-  </si>
-  <si>
-    <t>pnt_n67</t>
-  </si>
-  <si>
-    <t>pnt_n68</t>
-  </si>
-  <si>
-    <t>pnt_n69</t>
-  </si>
-  <si>
-    <t>pnt_n70</t>
-  </si>
-  <si>
-    <t>pnt_n71</t>
-  </si>
-  <si>
-    <t>pnt_n72</t>
-  </si>
-  <si>
-    <t>pnt_n73</t>
-  </si>
-  <si>
-    <t>pnt_n74</t>
-  </si>
-  <si>
-    <t>pnt_n75</t>
-  </si>
-  <si>
-    <t>pnt_n76</t>
-  </si>
-  <si>
-    <t>pnt_n77</t>
-  </si>
-  <si>
-    <t>pnt_n78</t>
-  </si>
-  <si>
-    <t>pnt_t79</t>
-  </si>
-  <si>
-    <t>pnt_t80</t>
-  </si>
-  <si>
-    <t>pnt_t81</t>
-  </si>
-  <si>
-    <t>pnt_t82</t>
-  </si>
-  <si>
-    <t>pnt_t83</t>
-  </si>
-  <si>
-    <t>pnt_t84</t>
-  </si>
-  <si>
-    <t>pnt_t85</t>
-  </si>
-  <si>
-    <t>pnt_t86</t>
-  </si>
-  <si>
-    <t>pnt_t87</t>
-  </si>
-  <si>
-    <t>pnt_t88</t>
-  </si>
-  <si>
-    <t>pnt_t89</t>
-  </si>
-  <si>
-    <t>pnt_t90</t>
-  </si>
-  <si>
-    <t>pnt_t91</t>
-  </si>
-  <si>
-    <t>pnt_t92</t>
-  </si>
-  <si>
-    <t>pnt_t93</t>
-  </si>
-  <si>
-    <t>pnt_t94</t>
-  </si>
-  <si>
-    <t>pnt_t95</t>
-  </si>
-  <si>
-    <t>pnt_t96</t>
-  </si>
-  <si>
-    <t>pnt_t97</t>
-  </si>
-  <si>
-    <t>pnt_t98</t>
-  </si>
-  <si>
-    <t>pnt_t99</t>
-  </si>
-  <si>
-    <t>pnt_t100</t>
-  </si>
-  <si>
-    <t>pnt_t101</t>
-  </si>
-  <si>
-    <t>pnt_t102</t>
-  </si>
-  <si>
-    <t>pnt_t103</t>
-  </si>
-  <si>
-    <t>pnt_t104</t>
-  </si>
-  <si>
-    <t>pnt_t105</t>
-  </si>
-  <si>
-    <t>pnt_t106</t>
-  </si>
-  <si>
-    <t>pnt_t107</t>
-  </si>
-  <si>
-    <t>pnt_t108</t>
-  </si>
-  <si>
-    <t>pnt_t109</t>
-  </si>
-  <si>
-    <t>pnt_t110</t>
-  </si>
-  <si>
-    <t>pnt_t111</t>
-  </si>
-  <si>
-    <t>pnt_t112</t>
-  </si>
-  <si>
-    <t>pnt_t113</t>
-  </si>
-  <si>
-    <t>pnt_t114</t>
-  </si>
-  <si>
-    <t>pnt_t115</t>
-  </si>
-  <si>
-    <t>pnt_t116</t>
-  </si>
-  <si>
-    <t>pnt_t117</t>
-  </si>
-  <si>
-    <t>pnt_t118</t>
-  </si>
-  <si>
-    <t>pnt_t119</t>
-  </si>
-  <si>
-    <t>pnt_t120</t>
-  </si>
-  <si>
-    <t>pnt_t121</t>
-  </si>
-  <si>
-    <t>pnt_t122</t>
-  </si>
-  <si>
-    <t>pnt_t123</t>
-  </si>
-  <si>
-    <t>pnt_t124</t>
-  </si>
-  <si>
-    <t>pnt_t125</t>
-  </si>
-  <si>
-    <t>pnt_t126</t>
-  </si>
-  <si>
-    <t>pnt_t127</t>
-  </si>
-  <si>
-    <t>pnt_t128</t>
-  </si>
-  <si>
-    <t>pnt_t129</t>
-  </si>
-  <si>
-    <t>pnt_t130</t>
-  </si>
-  <si>
     <t>id_pnt</t>
   </si>
   <si>
@@ -1234,6 +454,786 @@
   </si>
   <si>
     <t>Superar metas</t>
+  </si>
+  <si>
+    <t>ycox</t>
+  </si>
+  <si>
+    <t>yequ</t>
+  </si>
+  <si>
+    <t>ypro</t>
+  </si>
+  <si>
+    <t>yorg</t>
+  </si>
+  <si>
+    <t>ypay</t>
+  </si>
+  <si>
+    <t>ycon</t>
+  </si>
+  <si>
+    <t>yret</t>
+  </si>
+  <si>
+    <t>yrec</t>
+  </si>
+  <si>
+    <t>ycla</t>
+  </si>
+  <si>
+    <t>ylid</t>
+  </si>
+  <si>
+    <t>yrit</t>
+  </si>
+  <si>
+    <t>ycom</t>
+  </si>
+  <si>
+    <t>ycic</t>
+  </si>
+  <si>
+    <t>ycov</t>
+  </si>
+  <si>
+    <t>yent</t>
+  </si>
+  <si>
+    <t>yrev</t>
+  </si>
+  <si>
+    <t>yinn</t>
+  </si>
+  <si>
+    <t>yesp</t>
+  </si>
+  <si>
+    <t>yada</t>
+  </si>
+  <si>
+    <t>ytom</t>
+  </si>
+  <si>
+    <t>yimp</t>
+  </si>
+  <si>
+    <t>yemp</t>
+  </si>
+  <si>
+    <t>yrel</t>
+  </si>
+  <si>
+    <t>ycso</t>
+  </si>
+  <si>
+    <t>yser</t>
+  </si>
+  <si>
+    <t>ysup</t>
+  </si>
+  <si>
+    <t>ncox</t>
+  </si>
+  <si>
+    <t>nequ</t>
+  </si>
+  <si>
+    <t>npro</t>
+  </si>
+  <si>
+    <t>norg</t>
+  </si>
+  <si>
+    <t>npay</t>
+  </si>
+  <si>
+    <t>ncon</t>
+  </si>
+  <si>
+    <t>nret</t>
+  </si>
+  <si>
+    <t>nrec</t>
+  </si>
+  <si>
+    <t>ncla</t>
+  </si>
+  <si>
+    <t>nlid</t>
+  </si>
+  <si>
+    <t>nrit</t>
+  </si>
+  <si>
+    <t>ncom</t>
+  </si>
+  <si>
+    <t>ncic</t>
+  </si>
+  <si>
+    <t>ncov</t>
+  </si>
+  <si>
+    <t>nent</t>
+  </si>
+  <si>
+    <t>nrev</t>
+  </si>
+  <si>
+    <t>ninn</t>
+  </si>
+  <si>
+    <t>nesp</t>
+  </si>
+  <si>
+    <t>nada</t>
+  </si>
+  <si>
+    <t>ntom</t>
+  </si>
+  <si>
+    <t>nimp</t>
+  </si>
+  <si>
+    <t>nemp</t>
+  </si>
+  <si>
+    <t>nrel</t>
+  </si>
+  <si>
+    <t>ncso</t>
+  </si>
+  <si>
+    <t>nser</t>
+  </si>
+  <si>
+    <t>nsup</t>
+  </si>
+  <si>
+    <t>nncox</t>
+  </si>
+  <si>
+    <t>nnequ</t>
+  </si>
+  <si>
+    <t>nnpro</t>
+  </si>
+  <si>
+    <t>nnorg</t>
+  </si>
+  <si>
+    <t>nnpay</t>
+  </si>
+  <si>
+    <t>nncon</t>
+  </si>
+  <si>
+    <t>nnret</t>
+  </si>
+  <si>
+    <t>nnrec</t>
+  </si>
+  <si>
+    <t>nncla</t>
+  </si>
+  <si>
+    <t>nnlid</t>
+  </si>
+  <si>
+    <t>nnrit</t>
+  </si>
+  <si>
+    <t>nncom</t>
+  </si>
+  <si>
+    <t>nncic</t>
+  </si>
+  <si>
+    <t>nncov</t>
+  </si>
+  <si>
+    <t>nnent</t>
+  </si>
+  <si>
+    <t>nnrev</t>
+  </si>
+  <si>
+    <t>nninn</t>
+  </si>
+  <si>
+    <t>nnesp</t>
+  </si>
+  <si>
+    <t>nnada</t>
+  </si>
+  <si>
+    <t>nntom</t>
+  </si>
+  <si>
+    <t>nnimp</t>
+  </si>
+  <si>
+    <t>nnemp</t>
+  </si>
+  <si>
+    <t>nnrel</t>
+  </si>
+  <si>
+    <t>nncso</t>
+  </si>
+  <si>
+    <t>nnser</t>
+  </si>
+  <si>
+    <t>nnsup</t>
+  </si>
+  <si>
+    <t>tcox</t>
+  </si>
+  <si>
+    <t>tequ</t>
+  </si>
+  <si>
+    <t>tpro</t>
+  </si>
+  <si>
+    <t>torg</t>
+  </si>
+  <si>
+    <t>tpay</t>
+  </si>
+  <si>
+    <t>tcon</t>
+  </si>
+  <si>
+    <t>tret</t>
+  </si>
+  <si>
+    <t>trec</t>
+  </si>
+  <si>
+    <t>tcla</t>
+  </si>
+  <si>
+    <t>tlid</t>
+  </si>
+  <si>
+    <t>trit</t>
+  </si>
+  <si>
+    <t>tcom</t>
+  </si>
+  <si>
+    <t>tcic</t>
+  </si>
+  <si>
+    <t>tcov</t>
+  </si>
+  <si>
+    <t>tent</t>
+  </si>
+  <si>
+    <t>trev</t>
+  </si>
+  <si>
+    <t>tinn</t>
+  </si>
+  <si>
+    <t>tesp</t>
+  </si>
+  <si>
+    <t>tada</t>
+  </si>
+  <si>
+    <t>ttom</t>
+  </si>
+  <si>
+    <t>timp</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>trel</t>
+  </si>
+  <si>
+    <t>tcso</t>
+  </si>
+  <si>
+    <t>tser</t>
+  </si>
+  <si>
+    <t>tsup</t>
+  </si>
+  <si>
+    <t>ttcox</t>
+  </si>
+  <si>
+    <t>ttequ</t>
+  </si>
+  <si>
+    <t>ttpro</t>
+  </si>
+  <si>
+    <t>ttorg</t>
+  </si>
+  <si>
+    <t>ttpay</t>
+  </si>
+  <si>
+    <t>ttcon</t>
+  </si>
+  <si>
+    <t>ttret</t>
+  </si>
+  <si>
+    <t>ttrec</t>
+  </si>
+  <si>
+    <t>ttcla</t>
+  </si>
+  <si>
+    <t>ttlid</t>
+  </si>
+  <si>
+    <t>ttrit</t>
+  </si>
+  <si>
+    <t>ttcom</t>
+  </si>
+  <si>
+    <t>ttcic</t>
+  </si>
+  <si>
+    <t>ttcov</t>
+  </si>
+  <si>
+    <t>ttent</t>
+  </si>
+  <si>
+    <t>ttrev</t>
+  </si>
+  <si>
+    <t>ttinn</t>
+  </si>
+  <si>
+    <t>ttesp</t>
+  </si>
+  <si>
+    <t>ttada</t>
+  </si>
+  <si>
+    <t>tttom</t>
+  </si>
+  <si>
+    <t>ttimp</t>
+  </si>
+  <si>
+    <t>ttemp</t>
+  </si>
+  <si>
+    <t>ttrel</t>
+  </si>
+  <si>
+    <t>ttcso</t>
+  </si>
+  <si>
+    <t>ttser</t>
+  </si>
+  <si>
+    <t>ttsup</t>
+  </si>
+  <si>
+    <t>pnt_ycox</t>
+  </si>
+  <si>
+    <t>pnt_yequ</t>
+  </si>
+  <si>
+    <t>pnt_ypro</t>
+  </si>
+  <si>
+    <t>pnt_yorg</t>
+  </si>
+  <si>
+    <t>pnt_ypay</t>
+  </si>
+  <si>
+    <t>pnt_ycon</t>
+  </si>
+  <si>
+    <t>pnt_yret</t>
+  </si>
+  <si>
+    <t>pnt_yrec</t>
+  </si>
+  <si>
+    <t>pnt_ycla</t>
+  </si>
+  <si>
+    <t>pnt_ylid</t>
+  </si>
+  <si>
+    <t>pnt_yrit</t>
+  </si>
+  <si>
+    <t>pnt_ycom</t>
+  </si>
+  <si>
+    <t>pnt_ycic</t>
+  </si>
+  <si>
+    <t>pnt_ycov</t>
+  </si>
+  <si>
+    <t>pnt_yent</t>
+  </si>
+  <si>
+    <t>pnt_yrev</t>
+  </si>
+  <si>
+    <t>pnt_yinn</t>
+  </si>
+  <si>
+    <t>pnt_yesp</t>
+  </si>
+  <si>
+    <t>pnt_yada</t>
+  </si>
+  <si>
+    <t>pnt_ytom</t>
+  </si>
+  <si>
+    <t>pnt_yimp</t>
+  </si>
+  <si>
+    <t>pnt_yemp</t>
+  </si>
+  <si>
+    <t>pnt_yrel</t>
+  </si>
+  <si>
+    <t>pnt_ycso</t>
+  </si>
+  <si>
+    <t>pnt_yser</t>
+  </si>
+  <si>
+    <t>pnt_ysup</t>
+  </si>
+  <si>
+    <t>pnt_ncox</t>
+  </si>
+  <si>
+    <t>pnt_nequ</t>
+  </si>
+  <si>
+    <t>pnt_npro</t>
+  </si>
+  <si>
+    <t>pnt_norg</t>
+  </si>
+  <si>
+    <t>pnt_npay</t>
+  </si>
+  <si>
+    <t>pnt_ncon</t>
+  </si>
+  <si>
+    <t>pnt_nret</t>
+  </si>
+  <si>
+    <t>pnt_nrec</t>
+  </si>
+  <si>
+    <t>pnt_ncla</t>
+  </si>
+  <si>
+    <t>pnt_nlid</t>
+  </si>
+  <si>
+    <t>pnt_nrit</t>
+  </si>
+  <si>
+    <t>pnt_ncom</t>
+  </si>
+  <si>
+    <t>pnt_ncic</t>
+  </si>
+  <si>
+    <t>pnt_ncov</t>
+  </si>
+  <si>
+    <t>pnt_nent</t>
+  </si>
+  <si>
+    <t>pnt_nrev</t>
+  </si>
+  <si>
+    <t>pnt_ninn</t>
+  </si>
+  <si>
+    <t>pnt_nesp</t>
+  </si>
+  <si>
+    <t>pnt_nada</t>
+  </si>
+  <si>
+    <t>pnt_ntom</t>
+  </si>
+  <si>
+    <t>pnt_nimp</t>
+  </si>
+  <si>
+    <t>pnt_nemp</t>
+  </si>
+  <si>
+    <t>pnt_nrel</t>
+  </si>
+  <si>
+    <t>pnt_ncso</t>
+  </si>
+  <si>
+    <t>pnt_nser</t>
+  </si>
+  <si>
+    <t>pnt_nsup</t>
+  </si>
+  <si>
+    <t>pnt_nncox</t>
+  </si>
+  <si>
+    <t>pnt_nnequ</t>
+  </si>
+  <si>
+    <t>pnt_nnpro</t>
+  </si>
+  <si>
+    <t>pnt_nnorg</t>
+  </si>
+  <si>
+    <t>pnt_nnpay</t>
+  </si>
+  <si>
+    <t>pnt_nncon</t>
+  </si>
+  <si>
+    <t>pnt_nnret</t>
+  </si>
+  <si>
+    <t>pnt_nnrec</t>
+  </si>
+  <si>
+    <t>pnt_nncla</t>
+  </si>
+  <si>
+    <t>pnt_nnlid</t>
+  </si>
+  <si>
+    <t>pnt_nnrit</t>
+  </si>
+  <si>
+    <t>pnt_nncom</t>
+  </si>
+  <si>
+    <t>pnt_nncic</t>
+  </si>
+  <si>
+    <t>pnt_nncov</t>
+  </si>
+  <si>
+    <t>pnt_nnent</t>
+  </si>
+  <si>
+    <t>pnt_nnrev</t>
+  </si>
+  <si>
+    <t>pnt_nninn</t>
+  </si>
+  <si>
+    <t>pnt_nnesp</t>
+  </si>
+  <si>
+    <t>pnt_nnada</t>
+  </si>
+  <si>
+    <t>pnt_nntom</t>
+  </si>
+  <si>
+    <t>pnt_nnimp</t>
+  </si>
+  <si>
+    <t>pnt_nnemp</t>
+  </si>
+  <si>
+    <t>pnt_nnrel</t>
+  </si>
+  <si>
+    <t>pnt_nncso</t>
+  </si>
+  <si>
+    <t>pnt_nnser</t>
+  </si>
+  <si>
+    <t>pnt_nnsup</t>
+  </si>
+  <si>
+    <t>pnt_tcox</t>
+  </si>
+  <si>
+    <t>pnt_tequ</t>
+  </si>
+  <si>
+    <t>pnt_tpro</t>
+  </si>
+  <si>
+    <t>pnt_torg</t>
+  </si>
+  <si>
+    <t>pnt_tpay</t>
+  </si>
+  <si>
+    <t>pnt_tcon</t>
+  </si>
+  <si>
+    <t>pnt_tret</t>
+  </si>
+  <si>
+    <t>pnt_trec</t>
+  </si>
+  <si>
+    <t>pnt_tcla</t>
+  </si>
+  <si>
+    <t>pnt_tlid</t>
+  </si>
+  <si>
+    <t>pnt_trit</t>
+  </si>
+  <si>
+    <t>pnt_tcom</t>
+  </si>
+  <si>
+    <t>pnt_tcic</t>
+  </si>
+  <si>
+    <t>pnt_tcov</t>
+  </si>
+  <si>
+    <t>pnt_tent</t>
+  </si>
+  <si>
+    <t>pnt_trev</t>
+  </si>
+  <si>
+    <t>pnt_tinn</t>
+  </si>
+  <si>
+    <t>pnt_tesp</t>
+  </si>
+  <si>
+    <t>pnt_tada</t>
+  </si>
+  <si>
+    <t>pnt_ttom</t>
+  </si>
+  <si>
+    <t>pnt_timp</t>
+  </si>
+  <si>
+    <t>pnt_temp</t>
+  </si>
+  <si>
+    <t>pnt_trel</t>
+  </si>
+  <si>
+    <t>pnt_tcso</t>
+  </si>
+  <si>
+    <t>pnt_tser</t>
+  </si>
+  <si>
+    <t>pnt_tsup</t>
+  </si>
+  <si>
+    <t>pnt_ttcox</t>
+  </si>
+  <si>
+    <t>pnt_ttequ</t>
+  </si>
+  <si>
+    <t>pnt_ttpro</t>
+  </si>
+  <si>
+    <t>pnt_ttorg</t>
+  </si>
+  <si>
+    <t>pnt_ttpay</t>
+  </si>
+  <si>
+    <t>pnt_ttcon</t>
+  </si>
+  <si>
+    <t>pnt_ttret</t>
+  </si>
+  <si>
+    <t>pnt_ttrec</t>
+  </si>
+  <si>
+    <t>pnt_ttcla</t>
+  </si>
+  <si>
+    <t>pnt_ttlid</t>
+  </si>
+  <si>
+    <t>pnt_ttrit</t>
+  </si>
+  <si>
+    <t>pnt_ttcom</t>
+  </si>
+  <si>
+    <t>pnt_ttcic</t>
+  </si>
+  <si>
+    <t>pnt_ttcov</t>
+  </si>
+  <si>
+    <t>pnt_ttent</t>
+  </si>
+  <si>
+    <t>pnt_ttrev</t>
+  </si>
+  <si>
+    <t>pnt_ttinn</t>
+  </si>
+  <si>
+    <t>pnt_ttesp</t>
+  </si>
+  <si>
+    <t>pnt_ttada</t>
+  </si>
+  <si>
+    <t>pnt_tttom</t>
+  </si>
+  <si>
+    <t>pnt_ttimp</t>
+  </si>
+  <si>
+    <t>pnt_ttemp</t>
+  </si>
+  <si>
+    <t>pnt_ttrel</t>
+  </si>
+  <si>
+    <t>pnt_ttcso</t>
+  </si>
+  <si>
+    <t>pnt_ttser</t>
+  </si>
+  <si>
+    <t>pnt_ttsup</t>
   </si>
 </sst>
 </file>
@@ -1673,8 +1673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224B91BE-E32E-4506-A86E-9E3F6E02D172}">
   <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1696,538 +1696,538 @@
         <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>164</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>295</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>370</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>142</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C2" s="9">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>376</v>
+        <v>116</v>
       </c>
       <c r="E2" t="s">
-        <v>165</v>
+        <v>272</v>
       </c>
       <c r="F2" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>143</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C3" s="9">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>377</v>
+        <v>117</v>
       </c>
       <c r="E3" t="s">
-        <v>166</v>
+        <v>273</v>
       </c>
       <c r="F3" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>144</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C4" s="9">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>378</v>
+        <v>118</v>
       </c>
       <c r="E4" t="s">
-        <v>167</v>
+        <v>274</v>
       </c>
       <c r="F4" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>145</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C5" s="9">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>379</v>
+        <v>119</v>
       </c>
       <c r="E5" t="s">
-        <v>168</v>
+        <v>275</v>
       </c>
       <c r="F5" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>146</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C6" s="9">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>380</v>
+        <v>120</v>
       </c>
       <c r="E6" t="s">
-        <v>169</v>
+        <v>276</v>
       </c>
       <c r="F6" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>147</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C7" s="9">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>381</v>
+        <v>121</v>
       </c>
       <c r="E7" t="s">
-        <v>170</v>
+        <v>277</v>
       </c>
       <c r="F7" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>148</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C8" s="9">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>382</v>
+        <v>122</v>
       </c>
       <c r="E8" t="s">
-        <v>171</v>
+        <v>278</v>
       </c>
       <c r="F8" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>149</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C9" s="9">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>383</v>
+        <v>123</v>
       </c>
       <c r="E9" t="s">
-        <v>172</v>
+        <v>279</v>
       </c>
       <c r="F9" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>150</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C10" s="9">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>384</v>
+        <v>124</v>
       </c>
       <c r="E10" t="s">
-        <v>173</v>
+        <v>280</v>
       </c>
       <c r="F10" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>151</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C11" s="9">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>385</v>
+        <v>125</v>
       </c>
       <c r="E11" t="s">
-        <v>174</v>
+        <v>281</v>
       </c>
       <c r="F11" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>44</v>
+        <v>152</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C12" s="9">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>386</v>
+        <v>126</v>
       </c>
       <c r="E12" t="s">
-        <v>175</v>
+        <v>282</v>
       </c>
       <c r="F12" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>153</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C13" s="9">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>387</v>
+        <v>127</v>
       </c>
       <c r="E13" t="s">
-        <v>176</v>
+        <v>283</v>
       </c>
       <c r="F13" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>154</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C14" s="9">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>388</v>
+        <v>128</v>
       </c>
       <c r="E14" t="s">
-        <v>177</v>
+        <v>284</v>
       </c>
       <c r="F14" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>155</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C15" s="9">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>389</v>
+        <v>129</v>
       </c>
       <c r="E15" t="s">
-        <v>178</v>
+        <v>285</v>
       </c>
       <c r="F15" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>48</v>
+        <v>156</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C16" s="9">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>390</v>
+        <v>130</v>
       </c>
       <c r="E16" t="s">
-        <v>179</v>
+        <v>286</v>
       </c>
       <c r="F16" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>49</v>
+        <v>157</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C17" s="9">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>391</v>
+        <v>131</v>
       </c>
       <c r="E17" t="s">
-        <v>180</v>
+        <v>287</v>
       </c>
       <c r="F17" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>158</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C18" s="9">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>392</v>
+        <v>132</v>
       </c>
       <c r="E18" t="s">
-        <v>181</v>
+        <v>288</v>
       </c>
       <c r="F18" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>51</v>
+        <v>159</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C19" s="9">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>393</v>
+        <v>133</v>
       </c>
       <c r="E19" t="s">
-        <v>182</v>
+        <v>289</v>
       </c>
       <c r="F19" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>160</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C20" s="9">
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>394</v>
+        <v>134</v>
       </c>
       <c r="E20" t="s">
-        <v>183</v>
+        <v>290</v>
       </c>
       <c r="F20" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>53</v>
+        <v>161</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C21" s="9">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>395</v>
+        <v>135</v>
       </c>
       <c r="E21" t="s">
-        <v>184</v>
+        <v>291</v>
       </c>
       <c r="F21" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>54</v>
+        <v>162</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C22" s="9">
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>396</v>
+        <v>136</v>
       </c>
       <c r="E22" t="s">
-        <v>185</v>
+        <v>292</v>
       </c>
       <c r="F22" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>55</v>
+        <v>163</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C23" s="9">
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>397</v>
+        <v>137</v>
       </c>
       <c r="E23" t="s">
-        <v>186</v>
+        <v>293</v>
       </c>
       <c r="F23" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>164</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C24" s="9">
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>398</v>
+        <v>138</v>
       </c>
       <c r="E24" t="s">
-        <v>187</v>
+        <v>294</v>
       </c>
       <c r="F24" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>57</v>
+        <v>165</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C25" s="9">
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>399</v>
+        <v>139</v>
       </c>
       <c r="E25" t="s">
-        <v>188</v>
+        <v>295</v>
       </c>
       <c r="F25" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>58</v>
+        <v>166</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C26" s="9">
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>400</v>
+        <v>140</v>
       </c>
       <c r="E26" t="s">
-        <v>189</v>
+        <v>296</v>
       </c>
       <c r="F26" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>59</v>
+        <v>167</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="C27" s="9">
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>401</v>
+        <v>141</v>
       </c>
       <c r="E27" t="s">
-        <v>190</v>
+        <v>297</v>
       </c>
       <c r="F27" t="s">
-        <v>371</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>60</v>
+        <v>168</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>30</v>
@@ -2236,58 +2236,58 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>376</v>
+        <v>116</v>
       </c>
       <c r="E28" t="s">
-        <v>191</v>
+        <v>298</v>
       </c>
       <c r="F28" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>61</v>
+        <v>169</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>338</v>
+        <v>78</v>
       </c>
       <c r="C29" s="9">
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>377</v>
+        <v>117</v>
       </c>
       <c r="E29" t="s">
-        <v>192</v>
+        <v>299</v>
       </c>
       <c r="F29" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>62</v>
+        <v>170</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>296</v>
+        <v>36</v>
       </c>
       <c r="C30" s="9">
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>378</v>
+        <v>118</v>
       </c>
       <c r="E30" t="s">
-        <v>193</v>
+        <v>300</v>
       </c>
       <c r="F30" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>63</v>
+        <v>171</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>29</v>
@@ -2296,18 +2296,18 @@
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>379</v>
+        <v>119</v>
       </c>
       <c r="E31" t="s">
-        <v>194</v>
+        <v>301</v>
       </c>
       <c r="F31" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>28</v>
@@ -2316,18 +2316,18 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>380</v>
+        <v>120</v>
       </c>
       <c r="E32" t="s">
-        <v>195</v>
+        <v>302</v>
       </c>
       <c r="F32" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>65</v>
+        <v>173</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>27</v>
@@ -2336,38 +2336,38 @@
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>381</v>
+        <v>121</v>
       </c>
       <c r="E33" t="s">
-        <v>196</v>
+        <v>303</v>
       </c>
       <c r="F33" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>66</v>
+        <v>174</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>297</v>
+        <v>37</v>
       </c>
       <c r="C34" s="9">
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>382</v>
+        <v>122</v>
       </c>
       <c r="E34" t="s">
-        <v>197</v>
+        <v>304</v>
       </c>
       <c r="F34" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>67</v>
+        <v>175</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>26</v>
@@ -2376,58 +2376,58 @@
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>383</v>
+        <v>123</v>
       </c>
       <c r="E35" t="s">
-        <v>198</v>
+        <v>305</v>
       </c>
       <c r="F35" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>68</v>
+        <v>176</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>298</v>
+        <v>38</v>
       </c>
       <c r="C36" s="9">
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>384</v>
+        <v>124</v>
       </c>
       <c r="E36" t="s">
-        <v>199</v>
+        <v>306</v>
       </c>
       <c r="F36" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>69</v>
+        <v>177</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>345</v>
+        <v>85</v>
       </c>
       <c r="C37" s="9">
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>385</v>
+        <v>125</v>
       </c>
       <c r="E37" t="s">
-        <v>200</v>
+        <v>307</v>
       </c>
       <c r="F37" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>70</v>
+        <v>178</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>25</v>
@@ -2436,18 +2436,18 @@
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>386</v>
+        <v>126</v>
       </c>
       <c r="E38" t="s">
-        <v>201</v>
+        <v>308</v>
       </c>
       <c r="F38" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>71</v>
+        <v>179</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>24</v>
@@ -2456,18 +2456,18 @@
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>387</v>
+        <v>127</v>
       </c>
       <c r="E39" t="s">
-        <v>202</v>
+        <v>309</v>
       </c>
       <c r="F39" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>72</v>
+        <v>180</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>23</v>
@@ -2476,18 +2476,18 @@
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>388</v>
+        <v>128</v>
       </c>
       <c r="E40" t="s">
-        <v>203</v>
+        <v>310</v>
       </c>
       <c r="F40" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>73</v>
+        <v>181</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>22</v>
@@ -2496,78 +2496,78 @@
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>389</v>
+        <v>129</v>
       </c>
       <c r="E41" t="s">
-        <v>204</v>
+        <v>311</v>
       </c>
       <c r="F41" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>346</v>
+        <v>86</v>
       </c>
       <c r="C42" s="9">
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>390</v>
+        <v>130</v>
       </c>
       <c r="E42" t="s">
-        <v>205</v>
+        <v>312</v>
       </c>
       <c r="F42" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>75</v>
+        <v>183</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>299</v>
+        <v>39</v>
       </c>
       <c r="C43" s="9">
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>391</v>
+        <v>131</v>
       </c>
       <c r="E43" t="s">
-        <v>206</v>
+        <v>313</v>
       </c>
       <c r="F43" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>76</v>
+        <v>184</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>339</v>
+        <v>79</v>
       </c>
       <c r="C44" s="9">
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>392</v>
+        <v>132</v>
       </c>
       <c r="E44" t="s">
-        <v>207</v>
+        <v>314</v>
       </c>
       <c r="F44" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>77</v>
+        <v>185</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>21</v>
@@ -2576,18 +2576,18 @@
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>393</v>
+        <v>133</v>
       </c>
       <c r="E45" t="s">
-        <v>208</v>
+        <v>315</v>
       </c>
       <c r="F45" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>78</v>
+        <v>186</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>20</v>
@@ -2596,38 +2596,38 @@
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>394</v>
+        <v>134</v>
       </c>
       <c r="E46" t="s">
-        <v>209</v>
+        <v>316</v>
       </c>
       <c r="F46" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>79</v>
+        <v>187</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>347</v>
+        <v>87</v>
       </c>
       <c r="C47" s="9">
         <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>395</v>
+        <v>135</v>
       </c>
       <c r="E47" t="s">
-        <v>210</v>
+        <v>317</v>
       </c>
       <c r="F47" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>80</v>
+        <v>188</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>19</v>
@@ -2636,18 +2636,18 @@
         <v>0</v>
       </c>
       <c r="D48" t="s">
-        <v>396</v>
+        <v>136</v>
       </c>
       <c r="E48" t="s">
-        <v>211</v>
+        <v>318</v>
       </c>
       <c r="F48" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>81</v>
+        <v>189</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>18</v>
@@ -2656,18 +2656,18 @@
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>397</v>
+        <v>137</v>
       </c>
       <c r="E49" t="s">
-        <v>212</v>
+        <v>319</v>
       </c>
       <c r="F49" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>82</v>
+        <v>190</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>17</v>
@@ -2676,78 +2676,78 @@
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>398</v>
+        <v>138</v>
       </c>
       <c r="E50" t="s">
-        <v>213</v>
+        <v>320</v>
       </c>
       <c r="F50" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>83</v>
+        <v>191</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>300</v>
+        <v>40</v>
       </c>
       <c r="C51" s="9">
         <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>399</v>
+        <v>139</v>
       </c>
       <c r="E51" t="s">
-        <v>214</v>
+        <v>321</v>
       </c>
       <c r="F51" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>84</v>
+        <v>192</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>348</v>
+        <v>88</v>
       </c>
       <c r="C52" s="9">
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>400</v>
+        <v>140</v>
       </c>
       <c r="E52" t="s">
-        <v>215</v>
+        <v>322</v>
       </c>
       <c r="F52" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>85</v>
+        <v>193</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>349</v>
+        <v>89</v>
       </c>
       <c r="C53" s="9">
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>401</v>
+        <v>141</v>
       </c>
       <c r="E53" t="s">
-        <v>216</v>
+        <v>323</v>
       </c>
       <c r="F53" t="s">
-        <v>372</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>86</v>
+        <v>194</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>16</v>
@@ -2756,138 +2756,138 @@
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>376</v>
+        <v>116</v>
       </c>
       <c r="E54" t="s">
-        <v>217</v>
+        <v>324</v>
       </c>
       <c r="F54" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>301</v>
+        <v>41</v>
       </c>
       <c r="C55" s="9">
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>377</v>
+        <v>117</v>
       </c>
       <c r="E55" t="s">
-        <v>218</v>
+        <v>325</v>
       </c>
       <c r="F55" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>88</v>
+        <v>196</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>302</v>
+        <v>42</v>
       </c>
       <c r="C56" s="9">
         <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>378</v>
+        <v>118</v>
       </c>
       <c r="E56" t="s">
-        <v>219</v>
+        <v>326</v>
       </c>
       <c r="F56" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>89</v>
+        <v>197</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>303</v>
+        <v>43</v>
       </c>
       <c r="C57" s="9">
         <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>379</v>
+        <v>119</v>
       </c>
       <c r="E57" t="s">
-        <v>220</v>
+        <v>327</v>
       </c>
       <c r="F57" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>90</v>
+        <v>198</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>304</v>
+        <v>44</v>
       </c>
       <c r="C58" s="9">
         <v>0</v>
       </c>
       <c r="D58" t="s">
-        <v>380</v>
+        <v>120</v>
       </c>
       <c r="E58" t="s">
-        <v>221</v>
+        <v>328</v>
       </c>
       <c r="F58" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>91</v>
+        <v>199</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>340</v>
+        <v>80</v>
       </c>
       <c r="C59" s="9">
         <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>381</v>
+        <v>121</v>
       </c>
       <c r="E59" t="s">
-        <v>222</v>
+        <v>329</v>
       </c>
       <c r="F59" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>92</v>
+        <v>200</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>341</v>
+        <v>81</v>
       </c>
       <c r="C60" s="9">
         <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>382</v>
+        <v>122</v>
       </c>
       <c r="E60" t="s">
-        <v>223</v>
+        <v>330</v>
       </c>
       <c r="F60" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>93</v>
+        <v>201</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>15</v>
@@ -2896,18 +2896,18 @@
         <v>0</v>
       </c>
       <c r="D61" t="s">
-        <v>383</v>
+        <v>123</v>
       </c>
       <c r="E61" t="s">
-        <v>224</v>
+        <v>331</v>
       </c>
       <c r="F61" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>94</v>
+        <v>202</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>14</v>
@@ -2916,18 +2916,18 @@
         <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>384</v>
+        <v>124</v>
       </c>
       <c r="E62" t="s">
-        <v>225</v>
+        <v>332</v>
       </c>
       <c r="F62" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>95</v>
+        <v>203</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>13</v>
@@ -2936,58 +2936,58 @@
         <v>0</v>
       </c>
       <c r="D63" t="s">
-        <v>385</v>
+        <v>125</v>
       </c>
       <c r="E63" t="s">
-        <v>226</v>
+        <v>333</v>
       </c>
       <c r="F63" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>96</v>
+        <v>204</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>350</v>
+        <v>90</v>
       </c>
       <c r="C64" s="9">
         <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>386</v>
+        <v>126</v>
       </c>
       <c r="E64" t="s">
-        <v>227</v>
+        <v>334</v>
       </c>
       <c r="F64" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>97</v>
+        <v>205</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>305</v>
+        <v>45</v>
       </c>
       <c r="C65" s="9">
         <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>387</v>
+        <v>127</v>
       </c>
       <c r="E65" t="s">
-        <v>228</v>
+        <v>335</v>
       </c>
       <c r="F65" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>98</v>
+        <v>206</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>12</v>
@@ -2996,18 +2996,18 @@
         <v>0</v>
       </c>
       <c r="D66" t="s">
-        <v>388</v>
+        <v>128</v>
       </c>
       <c r="E66" t="s">
-        <v>229</v>
+        <v>336</v>
       </c>
       <c r="F66" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>99</v>
+        <v>207</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>11</v>
@@ -3016,78 +3016,78 @@
         <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>389</v>
+        <v>129</v>
       </c>
       <c r="E67" t="s">
-        <v>230</v>
+        <v>337</v>
       </c>
       <c r="F67" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>100</v>
+        <v>208</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>351</v>
+        <v>91</v>
       </c>
       <c r="C68" s="9">
         <v>0</v>
       </c>
       <c r="D68" t="s">
-        <v>390</v>
+        <v>130</v>
       </c>
       <c r="E68" t="s">
-        <v>231</v>
+        <v>338</v>
       </c>
       <c r="F68" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>101</v>
+        <v>209</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>342</v>
+        <v>82</v>
       </c>
       <c r="C69" s="9">
         <v>0</v>
       </c>
       <c r="D69" t="s">
-        <v>391</v>
+        <v>131</v>
       </c>
       <c r="E69" t="s">
-        <v>232</v>
+        <v>339</v>
       </c>
       <c r="F69" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>102</v>
+        <v>210</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>343</v>
+        <v>83</v>
       </c>
       <c r="C70" s="9">
         <v>1</v>
       </c>
       <c r="D70" t="s">
-        <v>392</v>
+        <v>132</v>
       </c>
       <c r="E70" t="s">
-        <v>233</v>
+        <v>340</v>
       </c>
       <c r="F70" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>103</v>
+        <v>211</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>10</v>
@@ -3096,18 +3096,18 @@
         <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>393</v>
+        <v>133</v>
       </c>
       <c r="E71" t="s">
-        <v>234</v>
+        <v>341</v>
       </c>
       <c r="F71" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>104</v>
+        <v>212</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>9</v>
@@ -3116,38 +3116,38 @@
         <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>394</v>
+        <v>134</v>
       </c>
       <c r="E72" t="s">
-        <v>235</v>
+        <v>342</v>
       </c>
       <c r="F72" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>105</v>
+        <v>213</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>344</v>
+        <v>84</v>
       </c>
       <c r="C73" s="9">
         <v>0</v>
       </c>
       <c r="D73" t="s">
-        <v>395</v>
+        <v>135</v>
       </c>
       <c r="E73" t="s">
-        <v>236</v>
+        <v>343</v>
       </c>
       <c r="F73" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>106</v>
+        <v>214</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>8</v>
@@ -3156,38 +3156,38 @@
         <v>1</v>
       </c>
       <c r="D74" t="s">
-        <v>396</v>
+        <v>136</v>
       </c>
       <c r="E74" t="s">
-        <v>237</v>
+        <v>344</v>
       </c>
       <c r="F74" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>107</v>
+        <v>215</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>352</v>
+        <v>92</v>
       </c>
       <c r="C75" s="9">
         <v>0</v>
       </c>
       <c r="D75" t="s">
-        <v>397</v>
+        <v>137</v>
       </c>
       <c r="E75" t="s">
-        <v>238</v>
+        <v>345</v>
       </c>
       <c r="F75" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>108</v>
+        <v>216</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>7</v>
@@ -3196,18 +3196,18 @@
         <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>398</v>
+        <v>138</v>
       </c>
       <c r="E76" t="s">
-        <v>239</v>
+        <v>346</v>
       </c>
       <c r="F76" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>109</v>
+        <v>217</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>6</v>
@@ -3216,18 +3216,18 @@
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>399</v>
+        <v>139</v>
       </c>
       <c r="E77" t="s">
-        <v>240</v>
+        <v>347</v>
       </c>
       <c r="F77" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>110</v>
+        <v>218</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>5</v>
@@ -3236,18 +3236,18 @@
         <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>400</v>
+        <v>140</v>
       </c>
       <c r="E78" t="s">
-        <v>241</v>
+        <v>348</v>
       </c>
       <c r="F78" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>111</v>
+        <v>219</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>4</v>
@@ -3256,318 +3256,318 @@
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>401</v>
+        <v>141</v>
       </c>
       <c r="E79" t="s">
-        <v>242</v>
+        <v>349</v>
       </c>
       <c r="F79" t="s">
-        <v>373</v>
+        <v>113</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>112</v>
+        <v>220</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>355</v>
+        <v>95</v>
       </c>
       <c r="C80" s="9">
         <v>0</v>
       </c>
       <c r="D80" t="s">
-        <v>376</v>
+        <v>116</v>
       </c>
       <c r="E80" t="s">
-        <v>243</v>
+        <v>350</v>
       </c>
       <c r="F80" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>113</v>
+        <v>221</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>306</v>
+        <v>46</v>
       </c>
       <c r="C81" s="9">
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>377</v>
+        <v>117</v>
       </c>
       <c r="E81" t="s">
-        <v>244</v>
+        <v>351</v>
       </c>
       <c r="F81" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C82" s="9">
+        <v>0</v>
+      </c>
+      <c r="D82" t="s">
+        <v>118</v>
+      </c>
+      <c r="E82" t="s">
+        <v>352</v>
+      </c>
+      <c r="F82" t="s">
         <v>114</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="C82" s="9">
-        <v>0</v>
-      </c>
-      <c r="D82" t="s">
-        <v>378</v>
-      </c>
-      <c r="E82" t="s">
-        <v>245</v>
-      </c>
-      <c r="F82" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>115</v>
+        <v>223</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>308</v>
+        <v>48</v>
       </c>
       <c r="C83" s="9">
         <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>379</v>
+        <v>119</v>
       </c>
       <c r="E83" t="s">
-        <v>246</v>
+        <v>353</v>
       </c>
       <c r="F83" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>116</v>
+        <v>224</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>309</v>
+        <v>49</v>
       </c>
       <c r="C84" s="9">
         <v>0</v>
       </c>
       <c r="D84" t="s">
-        <v>380</v>
+        <v>120</v>
       </c>
       <c r="E84" t="s">
-        <v>247</v>
+        <v>354</v>
       </c>
       <c r="F84" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>117</v>
+        <v>225</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>310</v>
+        <v>50</v>
       </c>
       <c r="C85" s="9">
         <v>0</v>
       </c>
       <c r="D85" t="s">
-        <v>381</v>
+        <v>121</v>
       </c>
       <c r="E85" t="s">
-        <v>248</v>
+        <v>355</v>
       </c>
       <c r="F85" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>118</v>
+        <v>226</v>
       </c>
       <c r="B86" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C86" s="9">
+        <v>0</v>
+      </c>
+      <c r="D86" t="s">
+        <v>122</v>
+      </c>
+      <c r="E86" t="s">
         <v>356</v>
       </c>
-      <c r="C86" s="9">
-        <v>0</v>
-      </c>
-      <c r="D86" t="s">
-        <v>382</v>
-      </c>
-      <c r="E86" t="s">
-        <v>249</v>
-      </c>
       <c r="F86" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>119</v>
+        <v>227</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>311</v>
+        <v>51</v>
       </c>
       <c r="C87" s="9">
         <v>0</v>
       </c>
       <c r="D87" t="s">
-        <v>383</v>
+        <v>123</v>
       </c>
       <c r="E87" t="s">
-        <v>250</v>
+        <v>357</v>
       </c>
       <c r="F87" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>120</v>
+        <v>228</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>357</v>
+        <v>97</v>
       </c>
       <c r="C88" s="9">
         <v>0</v>
       </c>
       <c r="D88" t="s">
-        <v>384</v>
+        <v>124</v>
       </c>
       <c r="E88" t="s">
-        <v>251</v>
+        <v>358</v>
       </c>
       <c r="F88" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>121</v>
+        <v>229</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>358</v>
+        <v>98</v>
       </c>
       <c r="C89" s="9">
         <v>0</v>
       </c>
       <c r="D89" t="s">
-        <v>385</v>
+        <v>125</v>
       </c>
       <c r="E89" t="s">
-        <v>252</v>
+        <v>359</v>
       </c>
       <c r="F89" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>122</v>
+        <v>230</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>312</v>
+        <v>52</v>
       </c>
       <c r="C90" s="9">
         <v>0</v>
       </c>
       <c r="D90" t="s">
-        <v>386</v>
+        <v>126</v>
       </c>
       <c r="E90" t="s">
-        <v>253</v>
+        <v>360</v>
       </c>
       <c r="F90" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>123</v>
+        <v>231</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>313</v>
+        <v>53</v>
       </c>
       <c r="C91" s="9">
         <v>0</v>
       </c>
       <c r="D91" t="s">
-        <v>387</v>
+        <v>127</v>
       </c>
       <c r="E91" t="s">
-        <v>254</v>
+        <v>361</v>
       </c>
       <c r="F91" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>124</v>
+        <v>232</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>314</v>
+        <v>54</v>
       </c>
       <c r="C92" s="9">
         <v>0</v>
       </c>
       <c r="D92" t="s">
-        <v>388</v>
+        <v>128</v>
       </c>
       <c r="E92" t="s">
-        <v>255</v>
+        <v>362</v>
       </c>
       <c r="F92" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>125</v>
+        <v>233</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>315</v>
+        <v>55</v>
       </c>
       <c r="C93" s="9">
         <v>0</v>
       </c>
       <c r="D93" t="s">
-        <v>389</v>
+        <v>129</v>
       </c>
       <c r="E93" t="s">
-        <v>256</v>
+        <v>363</v>
       </c>
       <c r="F93" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>126</v>
+        <v>234</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>359</v>
+        <v>99</v>
       </c>
       <c r="C94" s="9">
         <v>0</v>
       </c>
       <c r="D94" t="s">
-        <v>390</v>
+        <v>130</v>
       </c>
       <c r="E94" t="s">
-        <v>257</v>
+        <v>364</v>
       </c>
       <c r="F94" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>127</v>
+        <v>235</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>3</v>
@@ -3576,358 +3576,358 @@
         <v>0</v>
       </c>
       <c r="D95" t="s">
-        <v>391</v>
+        <v>131</v>
       </c>
       <c r="E95" t="s">
-        <v>258</v>
+        <v>365</v>
       </c>
       <c r="F95" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>128</v>
+        <v>236</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>360</v>
+        <v>100</v>
       </c>
       <c r="C96" s="9">
         <v>0</v>
       </c>
       <c r="D96" t="s">
-        <v>392</v>
+        <v>132</v>
       </c>
       <c r="E96" t="s">
-        <v>259</v>
+        <v>366</v>
       </c>
       <c r="F96" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>129</v>
+        <v>237</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>316</v>
+        <v>56</v>
       </c>
       <c r="C97" s="9">
         <v>0</v>
       </c>
       <c r="D97" t="s">
-        <v>393</v>
+        <v>133</v>
       </c>
       <c r="E97" t="s">
-        <v>260</v>
+        <v>367</v>
       </c>
       <c r="F97" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>130</v>
+        <v>238</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>317</v>
+        <v>57</v>
       </c>
       <c r="C98" s="9">
         <v>0</v>
       </c>
       <c r="D98" t="s">
-        <v>394</v>
+        <v>134</v>
       </c>
       <c r="E98" t="s">
-        <v>261</v>
+        <v>368</v>
       </c>
       <c r="F98" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>131</v>
+        <v>239</v>
       </c>
       <c r="B99" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C99" s="9">
+        <v>0</v>
+      </c>
+      <c r="D99" t="s">
+        <v>135</v>
+      </c>
+      <c r="E99" t="s">
         <v>369</v>
       </c>
-      <c r="C99" s="9">
-        <v>0</v>
-      </c>
-      <c r="D99" t="s">
-        <v>395</v>
-      </c>
-      <c r="E99" t="s">
-        <v>262</v>
-      </c>
       <c r="F99" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>132</v>
+        <v>240</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>318</v>
+        <v>58</v>
       </c>
       <c r="C100" s="9">
         <v>0</v>
       </c>
       <c r="D100" t="s">
-        <v>396</v>
+        <v>136</v>
       </c>
       <c r="E100" t="s">
-        <v>263</v>
+        <v>370</v>
       </c>
       <c r="F100" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>133</v>
+        <v>241</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>319</v>
+        <v>59</v>
       </c>
       <c r="C101" s="9">
         <v>0</v>
       </c>
       <c r="D101" t="s">
-        <v>397</v>
+        <v>137</v>
       </c>
       <c r="E101" t="s">
-        <v>264</v>
+        <v>371</v>
       </c>
       <c r="F101" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>134</v>
+        <v>242</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>320</v>
+        <v>60</v>
       </c>
       <c r="C102" s="9">
         <v>0</v>
       </c>
       <c r="D102" t="s">
-        <v>398</v>
+        <v>138</v>
       </c>
       <c r="E102" t="s">
-        <v>265</v>
+        <v>372</v>
       </c>
       <c r="F102" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>135</v>
+        <v>243</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>361</v>
+        <v>101</v>
       </c>
       <c r="C103" s="9">
         <v>0</v>
       </c>
       <c r="D103" t="s">
-        <v>399</v>
+        <v>139</v>
       </c>
       <c r="E103" t="s">
-        <v>266</v>
+        <v>373</v>
       </c>
       <c r="F103" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>136</v>
+        <v>244</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>321</v>
+        <v>61</v>
       </c>
       <c r="C104" s="9">
         <v>0</v>
       </c>
       <c r="D104" t="s">
-        <v>400</v>
+        <v>140</v>
       </c>
       <c r="E104" t="s">
-        <v>267</v>
+        <v>374</v>
       </c>
       <c r="F104" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>137</v>
+        <v>245</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>322</v>
+        <v>62</v>
       </c>
       <c r="C105" s="9">
         <v>0</v>
       </c>
       <c r="D105" t="s">
-        <v>401</v>
+        <v>141</v>
       </c>
       <c r="E105" t="s">
-        <v>268</v>
+        <v>375</v>
       </c>
       <c r="F105" t="s">
-        <v>374</v>
+        <v>114</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>138</v>
+        <v>246</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>323</v>
+        <v>63</v>
       </c>
       <c r="C106" s="9">
         <v>0</v>
       </c>
       <c r="D106" t="s">
+        <v>116</v>
+      </c>
+      <c r="E106" t="s">
         <v>376</v>
       </c>
-      <c r="E106" t="s">
-        <v>269</v>
-      </c>
       <c r="F106" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>139</v>
+        <v>247</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>324</v>
+        <v>64</v>
       </c>
       <c r="C107" s="9">
         <v>0</v>
       </c>
       <c r="D107" t="s">
+        <v>117</v>
+      </c>
+      <c r="E107" t="s">
         <v>377</v>
       </c>
-      <c r="E107" t="s">
-        <v>270</v>
-      </c>
       <c r="F107" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>140</v>
+        <v>248</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>362</v>
+        <v>102</v>
       </c>
       <c r="C108" s="9">
         <v>0</v>
       </c>
       <c r="D108" t="s">
+        <v>118</v>
+      </c>
+      <c r="E108" t="s">
         <v>378</v>
       </c>
-      <c r="E108" t="s">
-        <v>271</v>
-      </c>
       <c r="F108" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>141</v>
+        <v>249</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>353</v>
+        <v>93</v>
       </c>
       <c r="C109" s="9">
         <v>0</v>
       </c>
       <c r="D109" t="s">
+        <v>119</v>
+      </c>
+      <c r="E109" t="s">
         <v>379</v>
       </c>
-      <c r="E109" t="s">
-        <v>272</v>
-      </c>
       <c r="F109" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>142</v>
+        <v>250</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>325</v>
+        <v>65</v>
       </c>
       <c r="C110" s="9">
         <v>1</v>
       </c>
       <c r="D110" t="s">
+        <v>120</v>
+      </c>
+      <c r="E110" t="s">
         <v>380</v>
       </c>
-      <c r="E110" t="s">
-        <v>273</v>
-      </c>
       <c r="F110" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>143</v>
+        <v>251</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>326</v>
+        <v>66</v>
       </c>
       <c r="C111" s="9">
         <v>0</v>
       </c>
       <c r="D111" t="s">
+        <v>121</v>
+      </c>
+      <c r="E111" t="s">
         <v>381</v>
       </c>
-      <c r="E111" t="s">
-        <v>274</v>
-      </c>
       <c r="F111" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>144</v>
+        <v>252</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>363</v>
+        <v>103</v>
       </c>
       <c r="C112" s="9">
         <v>0</v>
       </c>
       <c r="D112" t="s">
+        <v>122</v>
+      </c>
+      <c r="E112" t="s">
         <v>382</v>
       </c>
-      <c r="E112" t="s">
-        <v>275</v>
-      </c>
       <c r="F112" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>145</v>
+        <v>253</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>2</v>
@@ -3936,38 +3936,38 @@
         <v>0</v>
       </c>
       <c r="D113" t="s">
+        <v>123</v>
+      </c>
+      <c r="E113" t="s">
         <v>383</v>
       </c>
-      <c r="E113" t="s">
-        <v>276</v>
-      </c>
       <c r="F113" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>146</v>
+        <v>254</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>327</v>
+        <v>67</v>
       </c>
       <c r="C114" s="9">
         <v>0</v>
       </c>
       <c r="D114" t="s">
+        <v>124</v>
+      </c>
+      <c r="E114" t="s">
         <v>384</v>
       </c>
-      <c r="E114" t="s">
-        <v>277</v>
-      </c>
       <c r="F114" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>147</v>
+        <v>255</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>1</v>
@@ -3976,18 +3976,18 @@
         <v>0</v>
       </c>
       <c r="D115" t="s">
+        <v>125</v>
+      </c>
+      <c r="E115" t="s">
         <v>385</v>
       </c>
-      <c r="E115" t="s">
-        <v>278</v>
-      </c>
       <c r="F115" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>148</v>
+        <v>256</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>0</v>
@@ -3996,313 +3996,313 @@
         <v>0</v>
       </c>
       <c r="D116" t="s">
+        <v>126</v>
+      </c>
+      <c r="E116" t="s">
         <v>386</v>
       </c>
-      <c r="E116" t="s">
-        <v>279</v>
-      </c>
       <c r="F116" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>149</v>
+        <v>257</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>328</v>
+        <v>68</v>
       </c>
       <c r="C117" s="9">
         <v>1</v>
       </c>
       <c r="D117" t="s">
+        <v>127</v>
+      </c>
+      <c r="E117" t="s">
         <v>387</v>
       </c>
-      <c r="E117" t="s">
-        <v>280</v>
-      </c>
       <c r="F117" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>150</v>
+        <v>258</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>364</v>
+        <v>104</v>
       </c>
       <c r="C118" s="9">
         <v>0</v>
       </c>
       <c r="D118" t="s">
+        <v>128</v>
+      </c>
+      <c r="E118" t="s">
         <v>388</v>
       </c>
-      <c r="E118" t="s">
-        <v>281</v>
-      </c>
       <c r="F118" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>151</v>
+        <v>259</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>365</v>
+        <v>105</v>
       </c>
       <c r="C119" s="9">
         <v>1</v>
       </c>
       <c r="D119" t="s">
+        <v>129</v>
+      </c>
+      <c r="E119" t="s">
         <v>389</v>
       </c>
-      <c r="E119" t="s">
-        <v>282</v>
-      </c>
       <c r="F119" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>152</v>
+        <v>260</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>354</v>
+        <v>94</v>
       </c>
       <c r="C120" s="9">
         <v>0</v>
       </c>
       <c r="D120" t="s">
+        <v>130</v>
+      </c>
+      <c r="E120" t="s">
         <v>390</v>
       </c>
-      <c r="E120" t="s">
-        <v>283</v>
-      </c>
       <c r="F120" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>153</v>
+        <v>261</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>329</v>
+        <v>69</v>
       </c>
       <c r="C121" s="9">
         <v>0</v>
       </c>
       <c r="D121" t="s">
+        <v>131</v>
+      </c>
+      <c r="E121" t="s">
         <v>391</v>
       </c>
-      <c r="E121" t="s">
-        <v>284</v>
-      </c>
       <c r="F121" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>154</v>
+        <v>262</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>366</v>
+        <v>106</v>
       </c>
       <c r="C122" s="9">
         <v>1</v>
       </c>
       <c r="D122" t="s">
+        <v>132</v>
+      </c>
+      <c r="E122" t="s">
         <v>392</v>
       </c>
-      <c r="E122" t="s">
-        <v>285</v>
-      </c>
       <c r="F122" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>155</v>
+        <v>263</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>330</v>
+        <v>70</v>
       </c>
       <c r="C123" s="9">
         <v>0</v>
       </c>
       <c r="D123" t="s">
+        <v>133</v>
+      </c>
+      <c r="E123" t="s">
         <v>393</v>
       </c>
-      <c r="E123" t="s">
-        <v>286</v>
-      </c>
       <c r="F123" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>156</v>
+        <v>264</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>331</v>
+        <v>71</v>
       </c>
       <c r="C124" s="9">
         <v>1</v>
       </c>
       <c r="D124" t="s">
+        <v>134</v>
+      </c>
+      <c r="E124" t="s">
         <v>394</v>
       </c>
-      <c r="E124" t="s">
-        <v>287</v>
-      </c>
       <c r="F124" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>157</v>
+        <v>265</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>332</v>
+        <v>72</v>
       </c>
       <c r="C125" s="9">
         <v>1</v>
       </c>
       <c r="D125" t="s">
+        <v>135</v>
+      </c>
+      <c r="E125" t="s">
         <v>395</v>
       </c>
-      <c r="E125" t="s">
-        <v>288</v>
-      </c>
       <c r="F125" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>158</v>
+        <v>266</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>333</v>
+        <v>73</v>
       </c>
       <c r="C126" s="9">
         <v>0</v>
       </c>
       <c r="D126" t="s">
+        <v>136</v>
+      </c>
+      <c r="E126" t="s">
         <v>396</v>
       </c>
-      <c r="E126" t="s">
-        <v>289</v>
-      </c>
       <c r="F126" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="127" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>159</v>
+        <v>267</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>367</v>
+        <v>107</v>
       </c>
       <c r="C127" s="9">
         <v>0</v>
       </c>
       <c r="D127" t="s">
+        <v>137</v>
+      </c>
+      <c r="E127" t="s">
         <v>397</v>
       </c>
-      <c r="E127" t="s">
-        <v>290</v>
-      </c>
       <c r="F127" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="128" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>160</v>
+        <v>268</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>334</v>
+        <v>74</v>
       </c>
       <c r="C128" s="9">
         <v>0</v>
       </c>
       <c r="D128" t="s">
+        <v>138</v>
+      </c>
+      <c r="E128" t="s">
         <v>398</v>
       </c>
-      <c r="E128" t="s">
-        <v>291</v>
-      </c>
       <c r="F128" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>161</v>
+        <v>269</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>335</v>
+        <v>75</v>
       </c>
       <c r="C129" s="9">
         <v>0</v>
       </c>
       <c r="D129" t="s">
+        <v>139</v>
+      </c>
+      <c r="E129" t="s">
         <v>399</v>
       </c>
-      <c r="E129" t="s">
-        <v>292</v>
-      </c>
       <c r="F129" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="130" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>162</v>
+        <v>270</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>336</v>
+        <v>76</v>
       </c>
       <c r="C130" s="9">
         <v>0</v>
       </c>
       <c r="D130" t="s">
+        <v>140</v>
+      </c>
+      <c r="E130" t="s">
         <v>400</v>
       </c>
-      <c r="E130" t="s">
-        <v>293</v>
-      </c>
       <c r="F130" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
     <row r="131" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>163</v>
+        <v>271</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>368</v>
+        <v>108</v>
       </c>
       <c r="C131" s="9">
         <v>0</v>
       </c>
       <c r="D131" t="s">
+        <v>141</v>
+      </c>
+      <c r="E131" t="s">
         <v>401</v>
       </c>
-      <c r="E131" t="s">
-        <v>294</v>
-      </c>
       <c r="F131" t="s">
-        <v>375</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>